<commit_message>
[Auto] Update teams and Events
</commit_message>
<xml_diff>
--- a/INSCRICAO DO NASA SPACE APPS 2025 (respostas).xlsx
+++ b/INSCRICAO DO NASA SPACE APPS 2025 (respostas).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5221" uniqueCount="2538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5371" uniqueCount="2613">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -7625,6 +7625,231 @@
   </si>
   <si>
     <t>Através de encaminhamento de e-mail pela coordenação do meu curso.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Júlii Marques Da Silva Santos </t>
+  </si>
+  <si>
+    <t>04716150135</t>
+  </si>
+  <si>
+    <t>Aparecida de Goiânia</t>
+  </si>
+  <si>
+    <t>designjulio2020@outlook.com</t>
+  </si>
+  <si>
+    <t>Fiquei sabendo por indicação de um colega que vai participar!</t>
+  </si>
+  <si>
+    <t>Gustavo Ramos</t>
+  </si>
+  <si>
+    <t>01918289638</t>
+  </si>
+  <si>
+    <t>guxtavoramoz@gmail.com</t>
+  </si>
+  <si>
+    <t>Igor Martins Cardoso</t>
+  </si>
+  <si>
+    <t>(34) 996445008</t>
+  </si>
+  <si>
+    <t>igor.martins@estudante.iftm.edu.br</t>
+  </si>
+  <si>
+    <t>Engenharia, Tecnologia e Programação, Arte e Design, Negócios e Finanças, Educação e Pesquisa</t>
+  </si>
+  <si>
+    <t>Incentivo de professores</t>
+  </si>
+  <si>
+    <t>Raquel Emillene</t>
+  </si>
+  <si>
+    <t>09952359454</t>
+  </si>
+  <si>
+    <t>sxemillene@gmail.com</t>
+  </si>
+  <si>
+    <t>Engenharia, Saúde e Ciências Biológicas, Tecnologia e Programação, Meio Ambiente, Impacto Social, Arte e Design, Linguagens e Criatividade</t>
+  </si>
+  <si>
+    <t>Jussara Coelho</t>
+  </si>
+  <si>
+    <t>08105993686</t>
+  </si>
+  <si>
+    <t>jussarapcoelho@gmail.com</t>
+  </si>
+  <si>
+    <t>Lucas silva de lucena</t>
+  </si>
+  <si>
+    <t>05193596150</t>
+  </si>
+  <si>
+    <t>Pires do Rio</t>
+  </si>
+  <si>
+    <t>lucasdelucenadev@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filipe Nascimento </t>
+  </si>
+  <si>
+    <t>filipeoficial33@gmail.com</t>
+  </si>
+  <si>
+    <t>Meio Ambiente, Arte e Design, Negócios e Finanças, Educação e Pesquisa, Linguagens e Criatividade</t>
+  </si>
+  <si>
+    <t>Grupo Zebu valley</t>
+  </si>
+  <si>
+    <t>Letícia Toledo de Souza Mendonça</t>
+  </si>
+  <si>
+    <t>leticiatsm@icloud.com</t>
+  </si>
+  <si>
+    <t>Por meio da Universidade Presbteriana Mackenzie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meirielly Santos </t>
+  </si>
+  <si>
+    <t>04153479128</t>
+  </si>
+  <si>
+    <t>meirielly.santos@educacao.mg.gov.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divulgação de estudantes </t>
+  </si>
+  <si>
+    <t>Renan Henrique de Oliveira Silveira</t>
+  </si>
+  <si>
+    <t>renanhenriq2020@outlook.com</t>
+  </si>
+  <si>
+    <t>Grupo de whatspp</t>
+  </si>
+  <si>
+    <t>Jean Carlos Rodrigues de Souza</t>
+  </si>
+  <si>
+    <t>(34) 998366552</t>
+  </si>
+  <si>
+    <t>jecrsouza@gmail.com</t>
+  </si>
+  <si>
+    <t>Projeto CosmoTupi</t>
+  </si>
+  <si>
+    <t>João Pedro Balugoli</t>
+  </si>
+  <si>
+    <t>jpedrobalugoli@gmail.com</t>
+  </si>
+  <si>
+    <t>instragran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carlos Eduardo Silva De Oliveira </t>
+  </si>
+  <si>
+    <t xml:space="preserve">706.509.471-50 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morrinhos Goiás </t>
+  </si>
+  <si>
+    <t>silvadeoliveira997@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por grupo de faculdade </t>
+  </si>
+  <si>
+    <t>Igor Souza Nascimento</t>
+  </si>
+  <si>
+    <t>09875173924</t>
+  </si>
+  <si>
+    <t>Criciúma</t>
+  </si>
+  <si>
+    <t>igor.fisica@outlook.com</t>
+  </si>
+  <si>
+    <t>Grupo de caça asteróides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabriel Sousa Ferreira </t>
+  </si>
+  <si>
+    <t xml:space="preserve">38 988633830 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">138.412.866-23 </t>
+  </si>
+  <si>
+    <t>ferreirasou.gabriell@gmail.com</t>
+  </si>
+  <si>
+    <t>Lucas Nastalli</t>
+  </si>
+  <si>
+    <t>(34)98868-7277</t>
+  </si>
+  <si>
+    <t>119.902.496-12</t>
+  </si>
+  <si>
+    <t>lucasnastalli@gmail.com</t>
+  </si>
+  <si>
+    <t>Docentes da UNIUBE</t>
+  </si>
+  <si>
+    <t>Victor Alves De Freitas</t>
+  </si>
+  <si>
+    <t>128.330.386-82</t>
+  </si>
+  <si>
+    <t>vitoralves59@gmail.com</t>
+  </si>
+  <si>
+    <t>Brenner Rodrigues dos Santos</t>
+  </si>
+  <si>
+    <t>08549403164</t>
+  </si>
+  <si>
+    <t>catalão - go</t>
+  </si>
+  <si>
+    <t>brennerrds@gmail.com</t>
+  </si>
+  <si>
+    <t>atraves de pessoas do meu curso na faculdade</t>
+  </si>
+  <si>
+    <t>Amanda Emanuelle Malaman Santana</t>
+  </si>
+  <si>
+    <t>109.736.956-09</t>
+  </si>
+  <si>
+    <t>amandaemanuelle30@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -7788,10 +8013,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -7799,13 +8024,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -7979,7 +8204,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L714" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L733" displayName="Form_Responses" name="Form_Responses" id="1">
   <tableColumns count="12">
     <tableColumn name="Carimbo de data/hora" id="1"/>
     <tableColumn name="Nome e Sobrenome:" id="2"/>
@@ -32736,22 +32961,687 @@
       </c>
     </row>
     <row r="713">
-      <c r="A713" s="11"/>
-      <c r="B713" s="12"/>
-      <c r="C713" s="12"/>
-      <c r="D713" s="12"/>
-      <c r="E713" s="12"/>
-      <c r="F713" s="12"/>
-      <c r="G713" s="12"/>
-      <c r="H713" s="13"/>
-      <c r="I713" s="12"/>
-      <c r="J713" s="14"/>
-      <c r="K713" s="14"/>
-      <c r="L713" s="15"/>
+      <c r="A713" s="18">
+        <v>45895.803355462966</v>
+      </c>
+      <c r="B713" s="19" t="s">
+        <v>2538</v>
+      </c>
+      <c r="D713" s="19">
+        <v>6.2998288904E10</v>
+      </c>
+      <c r="E713" s="29" t="s">
+        <v>2539</v>
+      </c>
+      <c r="F713" s="19" t="s">
+        <v>2540</v>
+      </c>
+      <c r="G713" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H713" s="20">
+        <v>36785.0</v>
+      </c>
+      <c r="I713" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J713" s="19" t="s">
+        <v>2541</v>
+      </c>
+      <c r="K713" s="19" t="s">
+        <v>419</v>
+      </c>
+      <c r="L713" s="31" t="s">
+        <v>2542</v>
+      </c>
     </row>
     <row r="714">
-      <c r="A714" s="33"/>
-      <c r="H714" s="34"/>
+      <c r="A714" s="23">
+        <v>45895.82413677083</v>
+      </c>
+      <c r="B714" s="24" t="s">
+        <v>2543</v>
+      </c>
+      <c r="D714" s="24">
+        <v>3.4999381017E10</v>
+      </c>
+      <c r="E714" s="28" t="s">
+        <v>2544</v>
+      </c>
+      <c r="F714" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G714" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H714" s="25">
+        <v>37461.0</v>
+      </c>
+      <c r="I714" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J714" s="24" t="s">
+        <v>2545</v>
+      </c>
+      <c r="K714" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="L714" s="30" t="s">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" s="18">
+        <v>45895.82570836805</v>
+      </c>
+      <c r="B715" s="19" t="s">
+        <v>2546</v>
+      </c>
+      <c r="D715" s="19" t="s">
+        <v>2547</v>
+      </c>
+      <c r="E715" s="19">
+        <v>7.0536942676E10</v>
+      </c>
+      <c r="F715" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G715" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="H715" s="20">
+        <v>39952.0</v>
+      </c>
+      <c r="I715" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="J715" s="19" t="s">
+        <v>2548</v>
+      </c>
+      <c r="K715" s="19" t="s">
+        <v>2549</v>
+      </c>
+      <c r="L715" s="31" t="s">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" s="23">
+        <v>45895.83993945602</v>
+      </c>
+      <c r="B716" s="24" t="s">
+        <v>2551</v>
+      </c>
+      <c r="D716" s="24">
+        <v>8.1983354272E10</v>
+      </c>
+      <c r="E716" s="28" t="s">
+        <v>2552</v>
+      </c>
+      <c r="F716" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G716" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H716" s="25">
+        <v>37299.0</v>
+      </c>
+      <c r="I716" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J716" s="24" t="s">
+        <v>2553</v>
+      </c>
+      <c r="K716" s="24" t="s">
+        <v>2554</v>
+      </c>
+      <c r="L716" s="30" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" s="18">
+        <v>45895.84188127315</v>
+      </c>
+      <c r="B717" s="19" t="s">
+        <v>2555</v>
+      </c>
+      <c r="D717" s="19">
+        <v>3.499231164E10</v>
+      </c>
+      <c r="E717" s="29" t="s">
+        <v>2556</v>
+      </c>
+      <c r="F717" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G717" s="19" t="s">
+        <v>830</v>
+      </c>
+      <c r="H717" s="20">
+        <v>32002.0</v>
+      </c>
+      <c r="I717" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J717" s="19" t="s">
+        <v>2557</v>
+      </c>
+      <c r="K717" s="19" t="s">
+        <v>1151</v>
+      </c>
+      <c r="L717" s="31" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" s="23">
+        <v>45895.846691388884</v>
+      </c>
+      <c r="B718" s="24" t="s">
+        <v>2558</v>
+      </c>
+      <c r="D718" s="24">
+        <v>6.4999910358E10</v>
+      </c>
+      <c r="E718" s="28" t="s">
+        <v>2559</v>
+      </c>
+      <c r="F718" s="24" t="s">
+        <v>2560</v>
+      </c>
+      <c r="G718" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H718" s="25">
+        <v>35703.0</v>
+      </c>
+      <c r="I718" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J718" s="24" t="s">
+        <v>2561</v>
+      </c>
+      <c r="K718" s="24" t="s">
+        <v>646</v>
+      </c>
+      <c r="L718" s="30" t="s">
+        <v>2332</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" s="18">
+        <v>45895.858101377315</v>
+      </c>
+      <c r="B719" s="19" t="s">
+        <v>2562</v>
+      </c>
+      <c r="D719" s="19">
+        <v>3.4992090094E10</v>
+      </c>
+      <c r="E719" s="19">
+        <v>1.7628006671E10</v>
+      </c>
+      <c r="F719" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="G719" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H719" s="20">
+        <v>38271.0</v>
+      </c>
+      <c r="I719" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J719" s="19" t="s">
+        <v>2563</v>
+      </c>
+      <c r="K719" s="19" t="s">
+        <v>2564</v>
+      </c>
+      <c r="L719" s="31" t="s">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" s="23">
+        <v>45895.86293121528</v>
+      </c>
+      <c r="B720" s="24" t="s">
+        <v>2566</v>
+      </c>
+      <c r="D720" s="24">
+        <v>1.1994458149E10</v>
+      </c>
+      <c r="E720" s="24">
+        <v>5.3805084803E10</v>
+      </c>
+      <c r="F720" s="24" t="s">
+        <v>658</v>
+      </c>
+      <c r="G720" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H720" s="25">
+        <v>39129.0</v>
+      </c>
+      <c r="I720" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J720" s="24" t="s">
+        <v>2567</v>
+      </c>
+      <c r="K720" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="L720" s="30" t="s">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" s="18">
+        <v>45895.87754210648</v>
+      </c>
+      <c r="B721" s="19" t="s">
+        <v>2569</v>
+      </c>
+      <c r="D721" s="19">
+        <v>6.4981385401E10</v>
+      </c>
+      <c r="E721" s="29" t="s">
+        <v>2570</v>
+      </c>
+      <c r="F721" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G721" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="H721" s="20">
+        <v>36131.0</v>
+      </c>
+      <c r="I721" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J721" s="19" t="s">
+        <v>2571</v>
+      </c>
+      <c r="K721" s="19" t="s">
+        <v>635</v>
+      </c>
+      <c r="L721" s="31" t="s">
+        <v>2572</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" s="23">
+        <v>45895.89110267361</v>
+      </c>
+      <c r="B722" s="24" t="s">
+        <v>2573</v>
+      </c>
+      <c r="D722" s="24">
+        <v>1.7988208523E10</v>
+      </c>
+      <c r="E722" s="24">
+        <v>4.7340387838E10</v>
+      </c>
+      <c r="F722" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G722" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H722" s="25">
+        <v>37694.0</v>
+      </c>
+      <c r="I722" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J722" s="24" t="s">
+        <v>2574</v>
+      </c>
+      <c r="K722" s="24" t="s">
+        <v>2281</v>
+      </c>
+      <c r="L722" s="30" t="s">
+        <v>2575</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" s="18">
+        <v>45895.8926055787</v>
+      </c>
+      <c r="B723" s="19" t="s">
+        <v>2576</v>
+      </c>
+      <c r="D723" s="19" t="s">
+        <v>2577</v>
+      </c>
+      <c r="E723" s="19">
+        <v>1.4666253688E10</v>
+      </c>
+      <c r="F723" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G723" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="H723" s="20">
+        <v>39701.0</v>
+      </c>
+      <c r="I723" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J723" s="19" t="s">
+        <v>2578</v>
+      </c>
+      <c r="K723" s="19" t="s">
+        <v>1509</v>
+      </c>
+      <c r="L723" s="31" t="s">
+        <v>2579</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" s="23">
+        <v>45895.89332924769</v>
+      </c>
+      <c r="B724" s="24" t="s">
+        <v>2580</v>
+      </c>
+      <c r="D724" s="24">
+        <v>1.6992105765E10</v>
+      </c>
+      <c r="E724" s="24">
+        <v>3.6408653839E10</v>
+      </c>
+      <c r="F724" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G724" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H724" s="25">
+        <v>38252.0</v>
+      </c>
+      <c r="I724" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J724" s="24" t="s">
+        <v>2581</v>
+      </c>
+      <c r="K724" s="24" t="s">
+        <v>444</v>
+      </c>
+      <c r="L724" s="30" t="s">
+        <v>2582</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" s="18">
+        <v>45895.894841284724</v>
+      </c>
+      <c r="B725" s="19" t="s">
+        <v>2583</v>
+      </c>
+      <c r="D725" s="19">
+        <v>6.4992039776E10</v>
+      </c>
+      <c r="E725" s="19" t="s">
+        <v>2584</v>
+      </c>
+      <c r="F725" s="19" t="s">
+        <v>2585</v>
+      </c>
+      <c r="G725" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H725" s="20">
+        <v>37673.0</v>
+      </c>
+      <c r="I725" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="J725" s="19" t="s">
+        <v>2586</v>
+      </c>
+      <c r="K725" s="19" t="s">
+        <v>444</v>
+      </c>
+      <c r="L725" s="31" t="s">
+        <v>2587</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" s="23">
+        <v>45895.93340180555</v>
+      </c>
+      <c r="B726" s="24" t="s">
+        <v>2588</v>
+      </c>
+      <c r="D726" s="24">
+        <v>4.8999246532E10</v>
+      </c>
+      <c r="E726" s="28" t="s">
+        <v>2589</v>
+      </c>
+      <c r="F726" s="24" t="s">
+        <v>2590</v>
+      </c>
+      <c r="G726" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H726" s="25">
+        <v>35851.0</v>
+      </c>
+      <c r="I726" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="J726" s="24" t="s">
+        <v>2591</v>
+      </c>
+      <c r="K726" s="24" t="s">
+        <v>1257</v>
+      </c>
+      <c r="L726" s="30" t="s">
+        <v>2592</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" s="18">
+        <v>45896.065861111114</v>
+      </c>
+      <c r="B727" s="19" t="s">
+        <v>2593</v>
+      </c>
+      <c r="D727" s="19" t="s">
+        <v>2594</v>
+      </c>
+      <c r="E727" s="19" t="s">
+        <v>2595</v>
+      </c>
+      <c r="F727" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G727" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H727" s="20">
+        <v>35863.0</v>
+      </c>
+      <c r="I727" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J727" s="19" t="s">
+        <v>2596</v>
+      </c>
+      <c r="K727" s="19" t="s">
+        <v>1399</v>
+      </c>
+      <c r="L727" s="31" t="s">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" s="23">
+        <v>45896.344786284724</v>
+      </c>
+      <c r="B728" s="24" t="s">
+        <v>2597</v>
+      </c>
+      <c r="D728" s="24" t="s">
+        <v>2598</v>
+      </c>
+      <c r="E728" s="24" t="s">
+        <v>2599</v>
+      </c>
+      <c r="F728" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="G728" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H728" s="25">
+        <v>39107.0</v>
+      </c>
+      <c r="I728" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J728" s="24" t="s">
+        <v>2600</v>
+      </c>
+      <c r="K728" s="24" t="s">
+        <v>1261</v>
+      </c>
+      <c r="L728" s="30" t="s">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" s="18">
+        <v>45896.34634336806</v>
+      </c>
+      <c r="B729" s="19" t="s">
+        <v>2602</v>
+      </c>
+      <c r="D729" s="19">
+        <v>3.4996767593E10</v>
+      </c>
+      <c r="E729" s="19" t="s">
+        <v>2603</v>
+      </c>
+      <c r="F729" s="19" t="s">
+        <v>1242</v>
+      </c>
+      <c r="G729" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="H729" s="20">
+        <v>35282.0</v>
+      </c>
+      <c r="I729" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J729" s="19" t="s">
+        <v>2604</v>
+      </c>
+      <c r="K729" s="19" t="s">
+        <v>438</v>
+      </c>
+      <c r="L729" s="31" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" s="23">
+        <v>45896.350624375</v>
+      </c>
+      <c r="B730" s="24" t="s">
+        <v>2605</v>
+      </c>
+      <c r="D730" s="24">
+        <v>6.4999772378E10</v>
+      </c>
+      <c r="E730" s="28" t="s">
+        <v>2606</v>
+      </c>
+      <c r="F730" s="24" t="s">
+        <v>2607</v>
+      </c>
+      <c r="G730" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H730" s="25">
+        <v>37913.0</v>
+      </c>
+      <c r="I730" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J730" s="24" t="s">
+        <v>2608</v>
+      </c>
+      <c r="K730" s="24" t="s">
+        <v>1403</v>
+      </c>
+      <c r="L730" s="30" t="s">
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" s="18">
+        <v>45896.35133297453</v>
+      </c>
+      <c r="B731" s="19" t="s">
+        <v>2610</v>
+      </c>
+      <c r="D731" s="19">
+        <v>3.4998740507E10</v>
+      </c>
+      <c r="E731" s="19" t="s">
+        <v>2611</v>
+      </c>
+      <c r="F731" s="19" t="s">
+        <v>1242</v>
+      </c>
+      <c r="G731" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H731" s="20">
+        <v>35338.0</v>
+      </c>
+      <c r="I731" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J731" s="19" t="s">
+        <v>2612</v>
+      </c>
+      <c r="K731" s="19" t="s">
+        <v>438</v>
+      </c>
+      <c r="L731" s="31" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" s="6"/>
+      <c r="B732" s="7"/>
+      <c r="C732" s="7"/>
+      <c r="D732" s="7"/>
+      <c r="E732" s="7"/>
+      <c r="F732" s="7"/>
+      <c r="G732" s="7"/>
+      <c r="H732" s="8"/>
+      <c r="I732" s="7"/>
+      <c r="J732" s="9"/>
+      <c r="K732" s="9"/>
+      <c r="L732" s="10"/>
+    </row>
+    <row r="733">
+      <c r="A733" s="33"/>
+      <c r="H733" s="34"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>